<commit_message>
fix bug with extra spaces on range iteration
</commit_message>
<xml_diff>
--- a/demo/report.xlsx
+++ b/demo/report.xlsx
@@ -546,7 +546,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -714,12 +714,12 @@
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="true">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="C12" s="1" t="s">
         <v>0</v>
       </c>
@@ -728,11 +728,11 @@
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="true">
-      <c r="A13" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>0</v>
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>0</v>
@@ -742,8 +742,8 @@
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="true">
-      <c r="A14" s="9" t="s">
-        <v>0</v>
+      <c r="A14" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>0</v>
@@ -755,12 +755,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" ht="15.75" customHeight="true">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>0</v>
+      <c r="B15" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>0</v>
@@ -769,577 +769,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" ht="15.75" customHeight="true">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>0</v>
+      <c r="B16" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" ht="15.75" customHeight="true">
-      <c r="A23" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" ht="15.75" customHeight="true">
-      <c r="A24" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" ht="15.75" customHeight="true">
-      <c r="A25" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" ht="15.75" customHeight="true">
-      <c r="A26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" ht="15.75" customHeight="true">
-      <c r="A27" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="true">
-      <c r="A28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" ht="15.75" customHeight="true">
-      <c r="A29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" ht="15.75" customHeight="true">
-      <c r="A30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" ht="15.75" customHeight="true">
-      <c r="A31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" ht="15.75" customHeight="true">
-      <c r="A32" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" ht="15.75" customHeight="true">
-      <c r="A34" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="true">
-      <c r="A35" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" ht="15.75" customHeight="true">
-      <c r="A36" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" ht="15.75" customHeight="true">
-      <c r="A37" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" ht="15.75" customHeight="true">
-      <c r="A38" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" ht="15.75" customHeight="true">
-      <c r="A39" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" ht="15.75" customHeight="true">
-      <c r="A40" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" ht="15.75" customHeight="true">
-      <c r="A41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" ht="15.75" customHeight="true">
-      <c r="A42" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" ht="15.75" customHeight="true">
-      <c r="A43" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" ht="15.75" customHeight="true">
-      <c r="A44" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" ht="15.75" customHeight="true">
-      <c r="A46" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" ht="15.75" customHeight="true">
-      <c r="A47" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" ht="15.75" customHeight="true">
-      <c r="A48" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" ht="15.75" customHeight="true">
-      <c r="A49" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" ht="15.75" customHeight="true">
-      <c r="A50" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" ht="15.75" customHeight="true">
-      <c r="A51" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" ht="15.75" customHeight="true">
-      <c r="A52" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" ht="15.75" customHeight="true">
-      <c r="A53" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" ht="15.75" customHeight="true">
-      <c r="A54" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" ht="15.75" customHeight="true">
-      <c r="A55" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D56" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>